<commit_message>
added checking for overlaps
</commit_message>
<xml_diff>
--- a/2_output/temp/actb_probes.xlsx
+++ b/2_output/temp/actb_probes.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\lab-projects\snail-probedesigner-test\2_output\temp\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -84,49 +79,49 @@
     <t>CCCACATAGGAGTCCTTCTAATGTTATCTT</t>
   </si>
   <si>
+    <t>ACTB_padlock_1</t>
+  </si>
+  <si>
+    <t>ACATTACCATTCCCACCATCACACCAATTATTACTGAAACATACACTAAAGATA</t>
+  </si>
+  <si>
+    <t>ACTB_splint_1</t>
+  </si>
+  <si>
+    <t>ACCCACATAGGAGTCCTTCTAATGTTATCTT</t>
+  </si>
+  <si>
     <t>ACTB_padlock_2</t>
   </si>
   <si>
-    <t>ACATTACCATTCCCACCATCACACCAATTATTACTGAAACATACACTAAAGATA</t>
+    <t>ACATTAACCCATTCCCACCATCACAATTATTACTGAAACATACACTAAAGATA</t>
   </si>
   <si>
     <t>ACTB_splint_2</t>
   </si>
   <si>
-    <t>ACCCACATAGGAGTCCTTCTAATGTTATCTT</t>
+    <t>CACCCACATAGGAGTCCTTAATGTTATCTT</t>
+  </si>
+  <si>
+    <t>ACTB_padlock_3</t>
+  </si>
+  <si>
+    <t>ACATTATTCTGACCCATTCCCACCAATTATTACTGAAACATACACTAAAGATA</t>
+  </si>
+  <si>
+    <t>ACTB_splint_3</t>
+  </si>
+  <si>
+    <t>CTCGTCACCCACATAGGATAATGTTATCTT</t>
   </si>
   <si>
     <t>ACTB_padlock_4</t>
   </si>
   <si>
-    <t>ACATTAACCCATTCCCACCATCACAATTATTACTGAAACATACACTAAAGATA</t>
+    <t>ACATTACCTTCTGACCCATTCCCAAATTATTACTGAAACATACACTAAAGATA</t>
   </si>
   <si>
     <t>ACTB_splint_4</t>
-  </si>
-  <si>
-    <t>CACCCACATAGGAGTCCTTAATGTTATCTT</t>
-  </si>
-  <si>
-    <t>ACTB_padlock_6</t>
-  </si>
-  <si>
-    <t>ACATTATTCTGACCCATTCCCACCAATTATTACTGAAACATACACTAAAGATA</t>
-  </si>
-  <si>
-    <t>ACTB_splint_6</t>
-  </si>
-  <si>
-    <t>CTCGTCACCCACATAGGATAATGTTATCTT</t>
-  </si>
-  <si>
-    <t>ACTB_padlock_8</t>
-  </si>
-  <si>
-    <t>ACATTACCTTCTGACCCATTCCCAAATTATTACTGAAACATACACTAAAGATA</t>
-  </si>
-  <si>
-    <t>ACTB_splint_8</t>
   </si>
   <si>
     <t>GCCTCGTCACCCACATAGTAATGTTATCTT</t>
@@ -135,8 +130,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -173,14 +168,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -227,7 +214,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -259,10 +246,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -294,7 +280,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -470,27 +455,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="42.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="51" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,7 +500,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -554,7 +526,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -577,7 +549,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -603,7 +575,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -626,7 +598,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -652,7 +624,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -675,7 +647,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -701,7 +673,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -724,7 +696,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -750,7 +722,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>12</v>
       </c>

</xml_diff>